<commit_message>
update - probably needs revoming
</commit_message>
<xml_diff>
--- a/data/evo.xlsx
+++ b/data/evo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eudald\Desktop\PO\EscolesCovid\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C3510B-4E73-46A7-8F58-1626617780C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB233FEA-DC73-4247-A61D-1CF2F6949E17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,9 +353,7 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>